<commit_message>
worked on forecast alligner
</commit_message>
<xml_diff>
--- a/output_df.xlsx
+++ b/output_df.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -523,7 +523,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SKU001</t>
+          <t>SKU_1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -532,30 +532,32 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>0.95</v>
+        <v>0.98</v>
       </c>
       <c r="E2" t="n">
-        <v>8.51</v>
+        <v>21.11</v>
       </c>
       <c r="F2" t="n">
-        <v>6.85</v>
+        <v>15.17</v>
       </c>
       <c r="G2" t="n">
-        <v>4.8</v>
+        <v>320859232292.6</v>
       </c>
       <c r="H2" t="n">
-        <v>0.42</v>
+        <v>-0.1</v>
       </c>
       <c r="I2" t="n">
-        <v>4.84</v>
+        <v>49.49</v>
       </c>
       <c r="J2" t="n">
-        <v>52</v>
-      </c>
-      <c r="K2" t="inlineStr"/>
+        <v>1641</v>
+      </c>
+      <c r="K2" t="n">
+        <v>93.58</v>
+      </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
@@ -563,14 +565,14 @@
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Forecast-based SS</t>
+          <t>Rule-based SS</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SKU001</t>
+          <t>SKU_1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -579,30 +581,32 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>0.95</v>
+        <v>0.98</v>
       </c>
       <c r="E3" t="n">
-        <v>9.74</v>
+        <v>21.96</v>
       </c>
       <c r="F3" t="n">
-        <v>7.92</v>
+        <v>14.93</v>
       </c>
       <c r="G3" t="n">
-        <v>6.96</v>
+        <v>289695307847.15</v>
       </c>
       <c r="H3" t="n">
-        <v>0.12</v>
+        <v>6.97</v>
       </c>
       <c r="I3" t="n">
-        <v>6.95</v>
+        <v>58.44</v>
       </c>
       <c r="J3" t="n">
-        <v>52</v>
-      </c>
-      <c r="K3" t="inlineStr"/>
+        <v>1641</v>
+      </c>
+      <c r="K3" t="n">
+        <v>78.63</v>
+      </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
@@ -610,97 +614,97 @@
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Forecast-based SS</t>
+          <t>Rule-based SS</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SKU002</t>
+          <t>SKU_1</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>DC</t>
+          <t>WH</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D4" t="n">
-        <v>0.95</v>
+        <v>0.98</v>
       </c>
       <c r="E4" t="n">
-        <v>12.02</v>
+        <v>27.86</v>
       </c>
       <c r="F4" t="n">
-        <v>10.25</v>
+        <v>18.79</v>
       </c>
       <c r="G4" t="n">
-        <v>5.12</v>
+        <v>263162705836.89</v>
       </c>
       <c r="H4" t="n">
-        <v>-1.75</v>
+        <v>12.28</v>
       </c>
       <c r="I4" t="n">
-        <v>5.09</v>
+        <v>73.23999999999999</v>
       </c>
       <c r="J4" t="n">
-        <v>52</v>
-      </c>
-      <c r="K4" t="inlineStr"/>
+        <v>1641</v>
+      </c>
+      <c r="K4" t="n">
+        <v>104.53</v>
+      </c>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
-      <c r="N4" t="n">
-        <v>85.8</v>
-      </c>
-      <c r="O4" t="n">
-        <v>1373.17</v>
-      </c>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Hybrid</t>
+          <t>Rule-based SS</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>SKU002</t>
+          <t>SKU_2</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Store</t>
+          <t>DC</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D5" t="n">
-        <v>0.95</v>
+        <v>0.98</v>
       </c>
       <c r="E5" t="n">
-        <v>9.34</v>
+        <v>20.65</v>
       </c>
       <c r="F5" t="n">
-        <v>7.4</v>
+        <v>12.75</v>
       </c>
       <c r="G5" t="n">
-        <v>5.62</v>
+        <v>106020719154.47</v>
       </c>
       <c r="H5" t="n">
-        <v>0.02</v>
+        <v>5.88</v>
       </c>
       <c r="I5" t="n">
-        <v>5.67</v>
+        <v>45.95</v>
       </c>
       <c r="J5" t="n">
-        <v>52</v>
-      </c>
-      <c r="K5" t="inlineStr"/>
+        <v>1641</v>
+      </c>
+      <c r="K5" t="n">
+        <v>152.29</v>
+      </c>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
@@ -708,46 +712,48 @@
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Forecast-based SS</t>
+          <t>Rule-based SS</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SKU003</t>
+          <t>SKU_2</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>DC</t>
+          <t>Store</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D6" t="n">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="E6" t="n">
-        <v>7.89</v>
+        <v>27.37</v>
       </c>
       <c r="F6" t="n">
-        <v>5.77</v>
+        <v>17.94</v>
       </c>
       <c r="G6" t="n">
-        <v>4.8</v>
+        <v>686142596112.72</v>
       </c>
       <c r="H6" t="n">
-        <v>0.42</v>
+        <v>12.41</v>
       </c>
       <c r="I6" t="n">
-        <v>4.89</v>
+        <v>73.11</v>
       </c>
       <c r="J6" t="n">
-        <v>52</v>
-      </c>
-      <c r="K6" t="inlineStr"/>
+        <v>1641</v>
+      </c>
+      <c r="K6" t="n">
+        <v>75.98</v>
+      </c>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
@@ -755,46 +761,48 @@
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Forecast-based SS</t>
+          <t>Rule-based SS</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>SKU003</t>
+          <t>SKU_2</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Store</t>
+          <t>WH</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" t="n">
-        <v>0.95</v>
+        <v>0.98</v>
       </c>
       <c r="E7" t="n">
-        <v>9.19</v>
+        <v>21.54</v>
       </c>
       <c r="F7" t="n">
-        <v>7.37</v>
+        <v>13.49</v>
       </c>
       <c r="G7" t="n">
-        <v>6.03</v>
+        <v>137093235897.45</v>
       </c>
       <c r="H7" t="n">
-        <v>0.06</v>
+        <v>-3.61</v>
       </c>
       <c r="I7" t="n">
-        <v>5.97</v>
+        <v>45.29</v>
       </c>
       <c r="J7" t="n">
-        <v>52</v>
-      </c>
-      <c r="K7" t="inlineStr"/>
+        <v>1641</v>
+      </c>
+      <c r="K7" t="n">
+        <v>124.81</v>
+      </c>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
@@ -802,7 +810,448 @@
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Forecast-based SS</t>
+          <t>Rule-based SS</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SKU_3</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>10</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="E8" t="n">
+        <v>18.25</v>
+      </c>
+      <c r="F8" t="n">
+        <v>12.84</v>
+      </c>
+      <c r="G8" t="n">
+        <v>340694698452.79</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-2.2</v>
+      </c>
+      <c r="I8" t="n">
+        <v>44.78</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1641</v>
+      </c>
+      <c r="K8" t="n">
+        <v>121.43</v>
+      </c>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>Rule-based SS</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>SKU_3</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Store</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>8</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="E9" t="n">
+        <v>25.25</v>
+      </c>
+      <c r="F9" t="n">
+        <v>14.13</v>
+      </c>
+      <c r="G9" t="n">
+        <v>17068860496.06</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-1.53</v>
+      </c>
+      <c r="I9" t="n">
+        <v>38.31</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1641</v>
+      </c>
+      <c r="K9" t="n">
+        <v>103.58</v>
+      </c>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>Rule-based SS</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>SKU_3</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>WH</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>17</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E10" t="n">
+        <v>22.15</v>
+      </c>
+      <c r="F10" t="n">
+        <v>14.02</v>
+      </c>
+      <c r="G10" t="n">
+        <v>42078001262.2</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-0.49</v>
+      </c>
+      <c r="I10" t="n">
+        <v>37.34</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1641</v>
+      </c>
+      <c r="K10" t="n">
+        <v>110.53</v>
+      </c>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>Rule-based SS</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>SKU_4</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>18</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="E11" t="n">
+        <v>23.44</v>
+      </c>
+      <c r="F11" t="n">
+        <v>15.79</v>
+      </c>
+      <c r="G11" t="n">
+        <v>45795246869.18</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="I11" t="n">
+        <v>49.98</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1641</v>
+      </c>
+      <c r="K11" t="n">
+        <v>125.47</v>
+      </c>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>Rule-based SS</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>SKU_4</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Store</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>18</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E12" t="n">
+        <v>23.56</v>
+      </c>
+      <c r="F12" t="n">
+        <v>15.38</v>
+      </c>
+      <c r="G12" t="n">
+        <v>167154174354.58</v>
+      </c>
+      <c r="H12" t="n">
+        <v>7.91</v>
+      </c>
+      <c r="I12" t="n">
+        <v>52.57</v>
+      </c>
+      <c r="J12" t="n">
+        <v>1641</v>
+      </c>
+      <c r="K12" t="n">
+        <v>92.89</v>
+      </c>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>Rule-based SS</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>SKU_4</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>WH</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>8</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="E13" t="n">
+        <v>18.88</v>
+      </c>
+      <c r="F13" t="n">
+        <v>11.87</v>
+      </c>
+      <c r="G13" t="n">
+        <v>128921389467.27</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="I13" t="n">
+        <v>43.4</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1641</v>
+      </c>
+      <c r="K13" t="n">
+        <v>78.41</v>
+      </c>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>Rule-based SS</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>SKU_5</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>8</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="E14" t="n">
+        <v>22.05</v>
+      </c>
+      <c r="F14" t="n">
+        <v>16.53</v>
+      </c>
+      <c r="G14" t="n">
+        <v>63924436405.61</v>
+      </c>
+      <c r="H14" t="n">
+        <v>5.85</v>
+      </c>
+      <c r="I14" t="n">
+        <v>57.42</v>
+      </c>
+      <c r="J14" t="n">
+        <v>1641</v>
+      </c>
+      <c r="K14" t="n">
+        <v>105.85</v>
+      </c>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>Rule-based SS</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>SKU_5</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Store</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>19</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="E15" t="n">
+        <v>27.52</v>
+      </c>
+      <c r="F15" t="n">
+        <v>17.69</v>
+      </c>
+      <c r="G15" t="n">
+        <v>90633759964.73</v>
+      </c>
+      <c r="H15" t="n">
+        <v>-11.17</v>
+      </c>
+      <c r="I15" t="n">
+        <v>44.08</v>
+      </c>
+      <c r="J15" t="n">
+        <v>1641</v>
+      </c>
+      <c r="K15" t="n">
+        <v>225.56</v>
+      </c>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr"/>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>Rule-based SS</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>SKU_5</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>WH</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>14</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E16" t="n">
+        <v>26.34</v>
+      </c>
+      <c r="F16" t="n">
+        <v>19.91</v>
+      </c>
+      <c r="G16" t="n">
+        <v>702199878302.3199</v>
+      </c>
+      <c r="H16" t="n">
+        <v>17.09</v>
+      </c>
+      <c r="I16" t="n">
+        <v>93.89</v>
+      </c>
+      <c r="J16" t="n">
+        <v>1641</v>
+      </c>
+      <c r="K16" t="n">
+        <v>62.49</v>
+      </c>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>Rule-based SS</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
modified the rule based approach
</commit_message>
<xml_diff>
--- a/output_df.xlsx
+++ b/output_df.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -532,32 +532,30 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D2" t="n">
-        <v>0.98</v>
+        <v>0.9</v>
       </c>
       <c r="E2" t="n">
-        <v>21.11</v>
+        <v>9.59</v>
       </c>
       <c r="F2" t="n">
-        <v>15.17</v>
+        <v>7.88</v>
       </c>
       <c r="G2" t="n">
-        <v>320859232292.6</v>
+        <v>4.24</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.1</v>
+        <v>1.64</v>
       </c>
       <c r="I2" t="n">
-        <v>49.49</v>
+        <v>4.24</v>
       </c>
       <c r="J2" t="n">
-        <v>1641</v>
-      </c>
-      <c r="K2" t="n">
-        <v>93.58</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
@@ -565,7 +563,7 @@
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Rule-based SS</t>
+          <t>Forecast-based SS</t>
         </is>
       </c>
     </row>
@@ -587,26 +585,24 @@
         <v>0.98</v>
       </c>
       <c r="E3" t="n">
-        <v>21.96</v>
+        <v>5.96</v>
       </c>
       <c r="F3" t="n">
-        <v>14.93</v>
+        <v>4.39</v>
       </c>
       <c r="G3" t="n">
-        <v>289695307847.15</v>
+        <v>4</v>
       </c>
       <c r="H3" t="n">
-        <v>6.97</v>
+        <v>0.04</v>
       </c>
       <c r="I3" t="n">
-        <v>58.44</v>
+        <v>4.08</v>
       </c>
       <c r="J3" t="n">
-        <v>1641</v>
-      </c>
-      <c r="K3" t="n">
-        <v>78.63</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
@@ -614,7 +610,7 @@
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Rule-based SS</t>
+          <t>Forecast-based SS</t>
         </is>
       </c>
     </row>
@@ -630,32 +626,30 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D4" t="n">
-        <v>0.98</v>
+        <v>0.95</v>
       </c>
       <c r="E4" t="n">
-        <v>27.86</v>
+        <v>10.02</v>
       </c>
       <c r="F4" t="n">
-        <v>18.79</v>
+        <v>8.140000000000001</v>
       </c>
       <c r="G4" t="n">
-        <v>263162705836.89</v>
+        <v>4.48</v>
       </c>
       <c r="H4" t="n">
-        <v>12.28</v>
+        <v>-0.38</v>
       </c>
       <c r="I4" t="n">
-        <v>73.23999999999999</v>
+        <v>4.58</v>
       </c>
       <c r="J4" t="n">
-        <v>1641</v>
-      </c>
-      <c r="K4" t="n">
-        <v>104.53</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
@@ -663,7 +657,7 @@
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Rule-based SS</t>
+          <t>Hybrid</t>
         </is>
       </c>
     </row>
@@ -679,31 +673,31 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D5" t="n">
-        <v>0.98</v>
+        <v>0.95</v>
       </c>
       <c r="E5" t="n">
-        <v>20.65</v>
+        <v>37.66</v>
       </c>
       <c r="F5" t="n">
-        <v>12.75</v>
+        <v>28.16</v>
       </c>
       <c r="G5" t="n">
-        <v>106020719154.47</v>
+        <v>12.15</v>
       </c>
       <c r="H5" t="n">
-        <v>5.88</v>
+        <v>-2.1</v>
       </c>
       <c r="I5" t="n">
-        <v>45.95</v>
+        <v>12.18</v>
       </c>
       <c r="J5" t="n">
-        <v>1641</v>
+        <v>104</v>
       </c>
       <c r="K5" t="n">
-        <v>152.29</v>
+        <v>267.61</v>
       </c>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
@@ -728,32 +722,30 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D6" t="n">
         <v>0.9</v>
       </c>
       <c r="E6" t="n">
-        <v>27.37</v>
+        <v>17.23</v>
       </c>
       <c r="F6" t="n">
-        <v>17.94</v>
+        <v>14.22</v>
       </c>
       <c r="G6" t="n">
-        <v>686142596112.72</v>
+        <v>12.19</v>
       </c>
       <c r="H6" t="n">
-        <v>12.41</v>
+        <v>-1.07</v>
       </c>
       <c r="I6" t="n">
-        <v>73.11</v>
+        <v>11.98</v>
       </c>
       <c r="J6" t="n">
-        <v>1641</v>
-      </c>
-      <c r="K6" t="n">
-        <v>75.98</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
@@ -761,7 +753,7 @@
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Rule-based SS</t>
+          <t>Hybrid</t>
         </is>
       </c>
     </row>
@@ -777,31 +769,31 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D7" t="n">
         <v>0.98</v>
       </c>
       <c r="E7" t="n">
-        <v>21.54</v>
+        <v>23.5</v>
       </c>
       <c r="F7" t="n">
-        <v>13.49</v>
+        <v>18.18</v>
       </c>
       <c r="G7" t="n">
-        <v>137093235897.45</v>
+        <v>12.04</v>
       </c>
       <c r="H7" t="n">
-        <v>-3.61</v>
+        <v>-1.64</v>
       </c>
       <c r="I7" t="n">
-        <v>45.29</v>
+        <v>11.71</v>
       </c>
       <c r="J7" t="n">
-        <v>1641</v>
+        <v>104</v>
       </c>
       <c r="K7" t="n">
-        <v>124.81</v>
+        <v>399.99</v>
       </c>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
@@ -826,31 +818,31 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D8" t="n">
         <v>0.98</v>
       </c>
       <c r="E8" t="n">
-        <v>18.25</v>
+        <v>40.64</v>
       </c>
       <c r="F8" t="n">
-        <v>12.84</v>
+        <v>34.66</v>
       </c>
       <c r="G8" t="n">
-        <v>340694698452.79</v>
+        <v>20.18</v>
       </c>
       <c r="H8" t="n">
-        <v>-2.2</v>
+        <v>33.49</v>
       </c>
       <c r="I8" t="n">
-        <v>44.78</v>
+        <v>20.31</v>
       </c>
       <c r="J8" t="n">
-        <v>1641</v>
+        <v>104</v>
       </c>
       <c r="K8" t="n">
-        <v>121.43</v>
+        <v>299.73</v>
       </c>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
@@ -875,31 +867,31 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D9" t="n">
         <v>0.95</v>
       </c>
       <c r="E9" t="n">
-        <v>25.25</v>
+        <v>25.33</v>
       </c>
       <c r="F9" t="n">
-        <v>14.13</v>
+        <v>21.86</v>
       </c>
       <c r="G9" t="n">
-        <v>17068860496.06</v>
+        <v>19.18</v>
       </c>
       <c r="H9" t="n">
-        <v>-1.53</v>
+        <v>21.27</v>
       </c>
       <c r="I9" t="n">
-        <v>38.31</v>
+        <v>19.46</v>
       </c>
       <c r="J9" t="n">
-        <v>1641</v>
+        <v>104</v>
       </c>
       <c r="K9" t="n">
-        <v>103.58</v>
+        <v>155.65</v>
       </c>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
@@ -924,31 +916,31 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D10" t="n">
         <v>0.9</v>
       </c>
       <c r="E10" t="n">
-        <v>22.15</v>
+        <v>40.55</v>
       </c>
       <c r="F10" t="n">
-        <v>14.02</v>
+        <v>34.14</v>
       </c>
       <c r="G10" t="n">
-        <v>42078001262.2</v>
+        <v>18.73</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.49</v>
+        <v>32.5</v>
       </c>
       <c r="I10" t="n">
-        <v>37.34</v>
+        <v>18.51</v>
       </c>
       <c r="J10" t="n">
-        <v>1641</v>
+        <v>104</v>
       </c>
       <c r="K10" t="n">
-        <v>110.53</v>
+        <v>182.2</v>
       </c>
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
@@ -973,31 +965,31 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" t="n">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="E11" t="n">
-        <v>23.44</v>
+        <v>52.81</v>
       </c>
       <c r="F11" t="n">
-        <v>15.79</v>
+        <v>44.03</v>
       </c>
       <c r="G11" t="n">
-        <v>45795246869.18</v>
+        <v>20.89</v>
       </c>
       <c r="H11" t="n">
-        <v>0.61</v>
+        <v>-43.09</v>
       </c>
       <c r="I11" t="n">
-        <v>49.98</v>
+        <v>20.58</v>
       </c>
       <c r="J11" t="n">
-        <v>1641</v>
+        <v>104</v>
       </c>
       <c r="K11" t="n">
-        <v>125.47</v>
+        <v>247.78</v>
       </c>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
@@ -1022,31 +1014,31 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9</v>
+        <v>0.98</v>
       </c>
       <c r="E12" t="n">
-        <v>23.56</v>
+        <v>23.14</v>
       </c>
       <c r="F12" t="n">
-        <v>15.38</v>
+        <v>19.39</v>
       </c>
       <c r="G12" t="n">
-        <v>167154174354.58</v>
+        <v>19.94</v>
       </c>
       <c r="H12" t="n">
-        <v>7.91</v>
+        <v>-18.96</v>
       </c>
       <c r="I12" t="n">
-        <v>52.57</v>
+        <v>19.66</v>
       </c>
       <c r="J12" t="n">
-        <v>1641</v>
+        <v>104</v>
       </c>
       <c r="K12" t="n">
-        <v>92.89</v>
+        <v>175.16</v>
       </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
@@ -1071,31 +1063,31 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D13" t="n">
         <v>0.95</v>
       </c>
       <c r="E13" t="n">
-        <v>18.88</v>
+        <v>38.29</v>
       </c>
       <c r="F13" t="n">
-        <v>11.87</v>
+        <v>32.98</v>
       </c>
       <c r="G13" t="n">
-        <v>128921389467.27</v>
+        <v>18.56</v>
       </c>
       <c r="H13" t="n">
-        <v>1.71</v>
+        <v>-32.2</v>
       </c>
       <c r="I13" t="n">
-        <v>43.4</v>
+        <v>18.2</v>
       </c>
       <c r="J13" t="n">
-        <v>1641</v>
+        <v>104</v>
       </c>
       <c r="K13" t="n">
-        <v>78.41</v>
+        <v>232.5</v>
       </c>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
@@ -1120,31 +1112,31 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" t="n">
-        <v>0.98</v>
+        <v>0.95</v>
       </c>
       <c r="E14" t="n">
-        <v>22.05</v>
+        <v>77.88</v>
       </c>
       <c r="F14" t="n">
-        <v>16.53</v>
+        <v>60.31</v>
       </c>
       <c r="G14" t="n">
-        <v>63924436405.61</v>
+        <v>28.75</v>
       </c>
       <c r="H14" t="n">
-        <v>5.85</v>
+        <v>1.96</v>
       </c>
       <c r="I14" t="n">
-        <v>57.42</v>
+        <v>28.48</v>
       </c>
       <c r="J14" t="n">
-        <v>1641</v>
+        <v>104</v>
       </c>
       <c r="K14" t="n">
-        <v>105.85</v>
+        <v>401.81</v>
       </c>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr"/>
@@ -1169,31 +1161,31 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="D15" t="n">
-        <v>0.98</v>
+        <v>0.9</v>
       </c>
       <c r="E15" t="n">
-        <v>27.52</v>
+        <v>46.1</v>
       </c>
       <c r="F15" t="n">
-        <v>17.69</v>
+        <v>36.15</v>
       </c>
       <c r="G15" t="n">
-        <v>90633759964.73</v>
+        <v>27.64</v>
       </c>
       <c r="H15" t="n">
-        <v>-11.17</v>
+        <v>1.12</v>
       </c>
       <c r="I15" t="n">
-        <v>44.08</v>
+        <v>27.81</v>
       </c>
       <c r="J15" t="n">
-        <v>1641</v>
+        <v>104</v>
       </c>
       <c r="K15" t="n">
-        <v>225.56</v>
+        <v>169.75</v>
       </c>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
@@ -1218,31 +1210,31 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D16" t="n">
-        <v>0.9</v>
+        <v>0.98</v>
       </c>
       <c r="E16" t="n">
-        <v>26.34</v>
+        <v>65.54000000000001</v>
       </c>
       <c r="F16" t="n">
-        <v>19.91</v>
+        <v>51.7</v>
       </c>
       <c r="G16" t="n">
-        <v>702199878302.3199</v>
+        <v>26.73</v>
       </c>
       <c r="H16" t="n">
-        <v>17.09</v>
+        <v>-11.27</v>
       </c>
       <c r="I16" t="n">
-        <v>93.89</v>
+        <v>27.02</v>
       </c>
       <c r="J16" t="n">
-        <v>1641</v>
+        <v>104</v>
       </c>
       <c r="K16" t="n">
-        <v>62.49</v>
+        <v>404.05</v>
       </c>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
@@ -1255,6 +1247,147 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>SKU_6</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>5</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="E17" t="n">
+        <v>14.19</v>
+      </c>
+      <c r="F17" t="n">
+        <v>11.45</v>
+      </c>
+      <c r="G17" t="n">
+        <v>4.65</v>
+      </c>
+      <c r="H17" t="n">
+        <v>-0.58</v>
+      </c>
+      <c r="I17" t="n">
+        <v>4.66</v>
+      </c>
+      <c r="J17" t="n">
+        <v>104</v>
+      </c>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>SKU_6</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Store</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>5</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="E18" t="n">
+        <v>4.85</v>
+      </c>
+      <c r="F18" t="n">
+        <v>3.82</v>
+      </c>
+      <c r="G18" t="n">
+        <v>3.66</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I18" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="J18" t="n">
+        <v>104</v>
+      </c>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>Forecast-based SS</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>SKU_6</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>WH</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>8</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E19" t="n">
+        <v>7.41</v>
+      </c>
+      <c r="F19" t="n">
+        <v>5.66</v>
+      </c>
+      <c r="G19" t="n">
+        <v>3.42</v>
+      </c>
+      <c r="H19" t="n">
+        <v>-0.38</v>
+      </c>
+      <c r="I19" t="n">
+        <v>3.46</v>
+      </c>
+      <c r="J19" t="n">
+        <v>104</v>
+      </c>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>Forecast-based SS</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>